<commit_message>
Added auto-save for last answer when time runs out in Quick Test
</commit_message>
<xml_diff>
--- a/questions5.xlsx
+++ b/questions5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D12C73-E06C-4ED9-B2B4-4CB7EA49A537}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DDC0C-757A-4070-9AEF-AAD519C772F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     <t>підривна машинка "Вихор-mini"</t>
   </si>
   <si>
-    <t>підривна машинка "Вихор"</t>
-  </si>
-  <si>
     <t>підривна машинка ПМ-4</t>
   </si>
   <si>
@@ -397,9 +394,6 @@
     <t>міна МОН-100</t>
   </si>
   <si>
-    <t>ПОМ-2</t>
-  </si>
-  <si>
     <t>Picture532</t>
   </si>
   <si>
@@ -568,9 +562,6 @@
     <t>міна МЗУ</t>
   </si>
   <si>
-    <t>міна МЗУ-2 "Верба"</t>
-  </si>
-  <si>
     <t>міна МЗС</t>
   </si>
   <si>
@@ -635,6 +626,15 @@
   </si>
   <si>
     <t>підривач УВЗ</t>
+  </si>
+  <si>
+    <t>підривна машинка Вихор</t>
+  </si>
+  <si>
+    <t>підривна машинка Вихор-mini</t>
+  </si>
+  <si>
+    <t>міна МЗУ-2 Верба</t>
   </si>
 </sst>
 </file>
@@ -926,8 +926,8 @@
   </sheetPr>
   <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA65" sqref="AA65"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1901,16 +1901,16 @@
         <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1921,7 +1921,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4" t="s">
-        <v>110</v>
+        <v>202</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -1952,16 +1952,16 @@
         <v>109</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="O21" s="3" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -1989,20 +1989,20 @@
         <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="H22" s="4"/>
       <c r="O22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2078,16 +2078,16 @@
         <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2098,7 +2098,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2126,19 +2126,19 @@
         <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="O25" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2166,19 +2166,19 @@
         <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="O26" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2206,19 +2206,19 @@
         <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="O27" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -2246,19 +2246,19 @@
         <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="O28" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
@@ -2286,19 +2286,19 @@
         <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="O29" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
@@ -2320,25 +2320,25 @@
     </row>
     <row r="30" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="O30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
@@ -2360,25 +2360,25 @@
     </row>
     <row r="31" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="O31" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
@@ -2400,25 +2400,25 @@
     </row>
     <row r="32" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="O32" s="2" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
@@ -2440,25 +2440,25 @@
     </row>
     <row r="33" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
@@ -2480,25 +2480,25 @@
     </row>
     <row r="34" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="O34" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
@@ -2520,25 +2520,25 @@
     </row>
     <row r="35" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="O35" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
@@ -2560,29 +2560,29 @@
     </row>
     <row r="36" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="O36" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
@@ -2600,29 +2600,29 @@
     </row>
     <row r="37" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="O37" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AA37" s="5" t="s">
         <v>35</v>
@@ -2633,25 +2633,25 @@
     </row>
     <row r="38" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="O38" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="AA38" s="5" t="s">
         <v>35</v>
@@ -2662,25 +2662,25 @@
     </row>
     <row r="39" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="O39" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AA39" s="5" t="s">
         <v>35</v>
@@ -2691,25 +2691,25 @@
     </row>
     <row r="40" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="O40" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AA40" s="5" t="s">
         <v>35</v>
@@ -2720,25 +2720,25 @@
     </row>
     <row r="41" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="O41" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AA41" s="5" t="s">
         <v>35</v>
@@ -2749,25 +2749,25 @@
     </row>
     <row r="42" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="O42" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AA42" s="5" t="s">
         <v>35</v>
@@ -2778,25 +2778,25 @@
     </row>
     <row r="43" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="O43" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AA43" s="5" t="s">
         <v>35</v>
@@ -2807,25 +2807,25 @@
     </row>
     <row r="44" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="O44" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AA44" s="5" t="s">
         <v>35</v>
@@ -2836,25 +2836,25 @@
     </row>
     <row r="45" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="F45" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA45" s="5" t="s">
         <v>35</v>
@@ -2865,25 +2865,25 @@
     </row>
     <row r="46" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="O46" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AA46" s="5" t="s">
         <v>35</v>
@@ -2894,25 +2894,25 @@
     </row>
     <row r="47" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="O47" s="2" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="AA47" s="5" t="s">
         <v>35</v>
@@ -2923,25 +2923,25 @@
     </row>
     <row r="48" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AA48" s="5" t="s">
         <v>35</v>
@@ -2952,25 +2952,25 @@
     </row>
     <row r="49" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O49" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AA49" s="5" t="s">
         <v>35</v>
@@ -2981,25 +2981,25 @@
     </row>
     <row r="50" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O50" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AA50" s="5" t="s">
         <v>35</v>
@@ -3010,25 +3010,25 @@
     </row>
     <row r="51" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AA51" s="5" t="s">
         <v>35</v>
@@ -3039,25 +3039,25 @@
     </row>
     <row r="52" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O52" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AA52" s="5" t="s">
         <v>35</v>
@@ -3068,25 +3068,25 @@
     </row>
     <row r="53" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AA53" s="5" t="s">
         <v>35</v>
@@ -3097,25 +3097,25 @@
     </row>
     <row r="54" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="O54" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AA54" s="5" t="s">
         <v>35</v>
@@ -3126,25 +3126,25 @@
     </row>
     <row r="55" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="O55" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AA55" s="5" t="s">
         <v>35</v>
@@ -3155,25 +3155,25 @@
     </row>
     <row r="56" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="O56" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AA56" s="5" t="s">
         <v>35</v>
@@ -3184,25 +3184,25 @@
     </row>
     <row r="57" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="O57" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AA57" s="5" t="s">
         <v>35</v>
@@ -3213,25 +3213,25 @@
     </row>
     <row r="58" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="O58" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AA58" s="5" t="s">
         <v>35</v>
@@ -3242,25 +3242,25 @@
     </row>
     <row r="59" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E59" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="O59" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AA59" s="5" t="s">
         <v>35</v>
@@ -3271,25 +3271,25 @@
     </row>
     <row r="60" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="O60" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AA60" s="5" t="s">
         <v>35</v>
@@ -3300,25 +3300,25 @@
     </row>
     <row r="61" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E61" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="O61" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AA61" s="5" t="s">
         <v>35</v>
@@ -3329,25 +3329,25 @@
     </row>
     <row r="62" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AA62" s="5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Fixed timer reset in Quick Test when clicking Next
</commit_message>
<xml_diff>
--- a/questions5.xlsx
+++ b/questions5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Программирование\test-with-password\alphatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DDC0C-757A-4070-9AEF-AAD519C772F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809C6904-DC59-4521-947A-C56832C72AB6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="204">
   <si>
     <t>Question</t>
   </si>
@@ -347,9 +347,6 @@
   </si>
   <si>
     <t>Picture528</t>
-  </si>
-  <si>
-    <t>підривна машинка "Вихор-mini"</t>
   </si>
   <si>
     <t>підривна машинка ПМ-4</t>
@@ -926,8 +923,8 @@
   </sheetPr>
   <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1901,16 +1898,16 @@
         <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1921,7 +1918,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -1949,19 +1946,19 @@
         <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -1989,20 +1986,20 @@
         <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="H22" s="4"/>
       <c r="O22" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2078,16 +2075,16 @@
         <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2098,7 +2095,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2126,19 +2123,19 @@
         <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="O25" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2166,19 +2163,19 @@
         <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="O26" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2206,19 +2203,19 @@
         <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="O27" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -2246,19 +2243,19 @@
         <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="O28" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
@@ -2286,19 +2283,19 @@
         <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="O29" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
@@ -2320,25 +2317,25 @@
     </row>
     <row r="30" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="O30" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
@@ -2360,25 +2357,25 @@
     </row>
     <row r="31" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="O31" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
@@ -2400,25 +2397,25 @@
     </row>
     <row r="32" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="O32" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
@@ -2440,25 +2437,25 @@
     </row>
     <row r="33" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
@@ -2480,25 +2477,25 @@
     </row>
     <row r="34" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="O34" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
@@ -2520,25 +2517,25 @@
     </row>
     <row r="35" spans="1:28" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="O35" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
@@ -2560,29 +2557,29 @@
     </row>
     <row r="36" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="O36" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
@@ -2600,29 +2597,29 @@
     </row>
     <row r="37" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="O37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA37" s="5" t="s">
         <v>35</v>
@@ -2633,25 +2630,25 @@
     </row>
     <row r="38" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="O38" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="AA38" s="5" t="s">
         <v>35</v>
@@ -2662,25 +2659,25 @@
     </row>
     <row r="39" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="O39" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AA39" s="5" t="s">
         <v>35</v>
@@ -2691,25 +2688,25 @@
     </row>
     <row r="40" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="O40" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AA40" s="5" t="s">
         <v>35</v>
@@ -2720,25 +2717,25 @@
     </row>
     <row r="41" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="O41" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AA41" s="5" t="s">
         <v>35</v>
@@ -2749,25 +2746,25 @@
     </row>
     <row r="42" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="O42" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AA42" s="5" t="s">
         <v>35</v>
@@ -2778,25 +2775,25 @@
     </row>
     <row r="43" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="O43" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA43" s="5" t="s">
         <v>35</v>
@@ -2807,25 +2804,25 @@
     </row>
     <row r="44" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="O44" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AA44" s="5" t="s">
         <v>35</v>
@@ -2836,25 +2833,25 @@
     </row>
     <row r="45" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="O45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AA45" s="5" t="s">
         <v>35</v>
@@ -2865,25 +2862,25 @@
     </row>
     <row r="46" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="O46" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AA46" s="5" t="s">
         <v>35</v>
@@ -2894,25 +2891,25 @@
     </row>
     <row r="47" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="O47" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AA47" s="5" t="s">
         <v>35</v>
@@ -2923,25 +2920,25 @@
     </row>
     <row r="48" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="O48" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA48" s="5" t="s">
         <v>35</v>
@@ -2952,25 +2949,25 @@
     </row>
     <row r="49" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="O49" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA49" s="5" t="s">
         <v>35</v>
@@ -2981,25 +2978,25 @@
     </row>
     <row r="50" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="O50" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AA50" s="5" t="s">
         <v>35</v>
@@ -3010,25 +3007,25 @@
     </row>
     <row r="51" spans="1:28" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F51" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA51" s="5" t="s">
         <v>35</v>
@@ -3039,25 +3036,25 @@
     </row>
     <row r="52" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="O52" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AA52" s="5" t="s">
         <v>35</v>
@@ -3068,25 +3065,25 @@
     </row>
     <row r="53" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O53" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA53" s="5" t="s">
         <v>35</v>
@@ -3097,25 +3094,25 @@
     </row>
     <row r="54" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="O54" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AA54" s="5" t="s">
         <v>35</v>
@@ -3126,25 +3123,25 @@
     </row>
     <row r="55" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="O55" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AA55" s="5" t="s">
         <v>35</v>
@@ -3155,25 +3152,25 @@
     </row>
     <row r="56" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="O56" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AA56" s="5" t="s">
         <v>35</v>
@@ -3184,25 +3181,25 @@
     </row>
     <row r="57" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="O57" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AA57" s="5" t="s">
         <v>35</v>
@@ -3213,25 +3210,25 @@
     </row>
     <row r="58" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="O58" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AA58" s="5" t="s">
         <v>35</v>
@@ -3242,25 +3239,25 @@
     </row>
     <row r="59" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="O59" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="AA59" s="5" t="s">
         <v>35</v>
@@ -3271,25 +3268,25 @@
     </row>
     <row r="60" spans="1:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="O60" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="AA60" s="5" t="s">
         <v>35</v>
@@ -3300,25 +3297,25 @@
     </row>
     <row r="61" spans="1:28" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="O61" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA61" s="5" t="s">
         <v>35</v>
@@ -3329,25 +3326,25 @@
     </row>
     <row r="62" spans="1:28" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="O62" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AA62" s="5" t="s">
         <v>35</v>

</xml_diff>